<commit_message>
[IMP] Add subtotal and total of payment amount
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_cd_receivable_balance_sheet_detail.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_cd_receivable_balance_sheet_detail.xlsx
@@ -255,6 +255,18 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <b val="1"/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+    </dxf>
+  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -475,6 +487,16 @@
       <c r="AMJ13" s="0"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A1:L1000000">
+    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>IF($A1="Subtotal",TRUE())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:L1000000">
+    <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>IF($A1="Total",TRUE())</formula>
+    </cfRule>
+  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>